<commit_message>
started working on biokart projeect and all files are uploaded
</commit_message>
<xml_diff>
--- a/biokart_website_automation/biokart_data.xlsx
+++ b/biokart_website_automation/biokart_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,8 +51,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -148,7 +156,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -180,9 +188,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,6 +223,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -389,16 +399,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,19 +419,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -429,7 +440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -443,7 +454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -457,7 +468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -481,12 +492,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>